<commit_message>
remove indexes from tables
</commit_message>
<xml_diff>
--- a/make_xl/data_xl/chairs.xlsx
+++ b/make_xl/data_xl/chairs.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Tabels\make_xl\data_xl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8A2770-3295-4015-A550-CF7D464E436E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -813,8 +807,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,26 +879,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -942,9 +928,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -976,27 +962,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1028,27 +996,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1221,1273 +1171,1334 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AM22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:39">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+    <row r="2" spans="1:39">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5000</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>99</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>102</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>103</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>112</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>113</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>117</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="3" spans="1:39">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5000</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>97</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>99</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>101</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>102</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>104</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>112</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>113</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>117</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="4" spans="1:39">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>15000</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>97</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>98</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>99</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>101</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>102</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>103</v>
       </c>
       <c r="AF4" t="s">
         <v>103</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AG4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI4" t="s">
         <v>112</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>114</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>117</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="1:39">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>57</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1499</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>97</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>98</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>100</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>101</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>102</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>105</v>
       </c>
       <c r="AF5" t="s">
         <v>105</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AG5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI5" t="s">
         <v>112</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>115</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>118</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="6" spans="1:39">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>58</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4000</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>97</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>98</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>99</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>101</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>102</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>106</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>112</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>113</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>117</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="7" spans="1:39">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2100</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>20379</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>97</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>98</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>99</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>101</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>102</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>107</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>112</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>113</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>118</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AM7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+    <row r="8" spans="1:39">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>60</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2499</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>20379</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>97</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>98</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>100</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>101</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>102</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>105</v>
       </c>
       <c r="AF8" t="s">
         <v>105</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AG8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI8" t="s">
         <v>112</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>115</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AK8" t="s">
         <v>118</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AM8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="9" spans="1:39">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>61</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2499</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>20379</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>97</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>98</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>100</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>101</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>102</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>105</v>
       </c>
       <c r="AF9" t="s">
         <v>105</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AG9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI9" t="s">
         <v>112</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AJ9" t="s">
         <v>115</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>118</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+    <row r="10" spans="1:39">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>62</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2099</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>20385</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>97</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>98</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>100</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>101</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>102</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>108</v>
       </c>
       <c r="AF10" t="s">
         <v>108</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AG10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI10" t="s">
         <v>112</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AJ10" t="s">
         <v>115</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AK10" t="s">
         <v>118</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AM10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="11" spans="1:39">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>63</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2999</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>20387</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>97</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>98</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>100</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>101</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>102</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>109</v>
       </c>
       <c r="AF11" t="s">
         <v>109</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AG11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI11" t="s">
         <v>112</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AJ11" t="s">
         <v>115</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AK11" t="s">
         <v>119</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AM11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="12" spans="1:39">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>64</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>3999</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>20391</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>97</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>98</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>100</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>101</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>102</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>109</v>
       </c>
       <c r="AF12" t="s">
         <v>109</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AG12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI12" t="s">
         <v>112</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AJ12" t="s">
         <v>115</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AK12" t="s">
         <v>118</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AM12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="13" spans="1:39">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>48</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>65</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>3499</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>20391</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>97</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>98</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>100</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>101</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>102</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>109</v>
       </c>
       <c r="AF13" t="s">
         <v>109</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AG13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI13" t="s">
         <v>112</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AJ13" t="s">
         <v>115</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AK13" t="s">
         <v>118</v>
       </c>
-      <c r="AL13" t="s">
+      <c r="AM13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="14" spans="1:39">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>49</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>66</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>4999</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>20433</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>97</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>98</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>100</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>101</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>102</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>109</v>
       </c>
       <c r="AF14" t="s">
         <v>109</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AG14" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI14" t="s">
         <v>112</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AJ14" t="s">
         <v>115</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AK14" t="s">
         <v>118</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AM14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="15" spans="1:39">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>67</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>5000</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>20433</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>97</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>98</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>99</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>101</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>102</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AF15" t="s">
         <v>109</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AI15" t="s">
         <v>112</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AJ15" t="s">
         <v>116</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AK15" t="s">
         <v>118</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AM15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+    <row r="16" spans="1:39">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>68</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>6999</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>20446</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>97</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>98</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>100</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>101</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>102</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>109</v>
       </c>
       <c r="AF16" t="s">
         <v>109</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AG16" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI16" t="s">
         <v>112</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AJ16" t="s">
         <v>113</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AK16" t="s">
         <v>120</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="AM16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="17" spans="1:39">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
         <v>43</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>69</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>4999</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>20446</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>97</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AB17" t="s">
         <v>98</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>100</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AD17" t="s">
         <v>101</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>102</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>110</v>
       </c>
       <c r="AF17" t="s">
         <v>110</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AG17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI17" t="s">
         <v>112</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AJ17" t="s">
         <v>113</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AK17" t="s">
         <v>120</v>
       </c>
-      <c r="AL17" t="s">
+      <c r="AM17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+    <row r="18" spans="1:39">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>70</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>3999</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>20455</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>97</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>98</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AC18" t="s">
         <v>100</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>101</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>102</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>109</v>
       </c>
       <c r="AF18" t="s">
         <v>109</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AG18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI18" t="s">
         <v>112</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AJ18" t="s">
         <v>115</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AK18" t="s">
         <v>118</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AM18" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+    <row r="19" spans="1:39">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
         <v>53</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>71</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>3999</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>20455</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>97</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AB19" t="s">
         <v>98</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>100</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>101</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>102</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>109</v>
       </c>
       <c r="AF19" t="s">
         <v>109</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AG19" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI19" t="s">
         <v>112</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AJ19" t="s">
         <v>115</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AK19" t="s">
         <v>118</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AM19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+    <row r="20" spans="1:39">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>72</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>5999</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>20457</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>97</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AB20" t="s">
         <v>98</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>100</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>101</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>102</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>104</v>
       </c>
       <c r="AF20" t="s">
         <v>104</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AG20" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI20" t="s">
         <v>112</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AJ20" t="s">
         <v>113</v>
       </c>
-      <c r="AJ20" t="s">
+      <c r="AK20" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" t="s">
+      <c r="AM20" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="21" spans="1:39">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
         <v>43</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>73</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>4999</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>20462</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>97</v>
       </c>
-      <c r="AA21" t="s">
+      <c r="AB21" t="s">
         <v>98</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AC21" t="s">
         <v>100</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AD21" t="s">
         <v>101</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>102</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>111</v>
       </c>
       <c r="AF21" t="s">
         <v>111</v>
       </c>
-      <c r="AH21" t="s">
+      <c r="AG21" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI21" t="s">
         <v>112</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AJ21" t="s">
         <v>113</v>
       </c>
-      <c r="AJ21" t="s">
+      <c r="AK21" t="s">
         <v>118</v>
       </c>
-      <c r="AL21" t="s">
+      <c r="AM21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="4:38" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="22" spans="1:39">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
         <v>46</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>74</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>4999</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>20463</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>97</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>98</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
         <v>100</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>101</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>102</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>107</v>
       </c>
       <c r="AF22" t="s">
         <v>107</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AG22" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI22" t="s">
         <v>112</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AJ22" t="s">
         <v>113</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AK22" t="s">
         <v>120</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AM22" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="I4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="I6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="I9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="I10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="I11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="I12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="I13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="I14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="I15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="I16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="I17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="I18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="I19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="G20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="I20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="G21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="I21" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="G22" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="I22" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId4"/>
+    <hyperlink ref="H4" r:id="rId5"/>
+    <hyperlink ref="J4" r:id="rId6"/>
+    <hyperlink ref="H5" r:id="rId7"/>
+    <hyperlink ref="J5" r:id="rId8"/>
+    <hyperlink ref="H6" r:id="rId9"/>
+    <hyperlink ref="J6" r:id="rId10"/>
+    <hyperlink ref="H7" r:id="rId11"/>
+    <hyperlink ref="J7" r:id="rId12"/>
+    <hyperlink ref="H8" r:id="rId13"/>
+    <hyperlink ref="J8" r:id="rId14"/>
+    <hyperlink ref="H9" r:id="rId15"/>
+    <hyperlink ref="J9" r:id="rId16"/>
+    <hyperlink ref="H10" r:id="rId17"/>
+    <hyperlink ref="J10" r:id="rId18"/>
+    <hyperlink ref="H11" r:id="rId19"/>
+    <hyperlink ref="J11" r:id="rId20"/>
+    <hyperlink ref="H12" r:id="rId21"/>
+    <hyperlink ref="J12" r:id="rId22"/>
+    <hyperlink ref="H13" r:id="rId23"/>
+    <hyperlink ref="J13" r:id="rId24"/>
+    <hyperlink ref="H14" r:id="rId25"/>
+    <hyperlink ref="J14" r:id="rId26"/>
+    <hyperlink ref="H15" r:id="rId27"/>
+    <hyperlink ref="J15" r:id="rId28"/>
+    <hyperlink ref="H16" r:id="rId29"/>
+    <hyperlink ref="J16" r:id="rId30"/>
+    <hyperlink ref="H17" r:id="rId31"/>
+    <hyperlink ref="J17" r:id="rId32"/>
+    <hyperlink ref="H18" r:id="rId33"/>
+    <hyperlink ref="J18" r:id="rId34"/>
+    <hyperlink ref="H19" r:id="rId35"/>
+    <hyperlink ref="J19" r:id="rId36"/>
+    <hyperlink ref="H20" r:id="rId37"/>
+    <hyperlink ref="J20" r:id="rId38"/>
+    <hyperlink ref="H21" r:id="rId39"/>
+    <hyperlink ref="J21" r:id="rId40"/>
+    <hyperlink ref="H22" r:id="rId41"/>
+    <hyperlink ref="J22" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>